<commit_message>
Readme update Reflexion und Bewertungsraster
</commit_message>
<xml_diff>
--- a/LB3/M300-LB3-Bewertungsraster-Protected.xlsx
+++ b/LB3/M300-LB3-Bewertungsraster-Protected.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tbzedu-my.sharepoint.com/personal/philipp_rohr_tbz_ch/Documents/Home/TBZ/02_Module/Modul 300/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thars\M300T\LB3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{CC54384D-0422-426E-B51C-904A7167611B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{526C2C28-023F-44CB-A7B7-00728A101249}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003297F8-5F03-4C64-81AD-B677B745642B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DocT7tNvssGLFBYor3T47R6qJ5I+CO88IurmOU4bJOCL+BFCH1qOCRKW6wfOy8pITSpMoi4A/Dq5eFihrc7pLw==" workbookSaltValue="DoD6xfmqCtYjjpTY+px99w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M262 - Fallstudie LB2" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,9 @@
   <commentList>
     <comment ref="C2" authorId="0" shapeId="0" xr:uid="{FFABAE7A-E58C-4405-A877-A44658A6DD81}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     4 P. = Es sind mehr als vier Kriterien erfüllt
 3 P. = Es sind drei Kriterien erfüllt
 2 P. = Es sind zwei Kriterien erfüllt
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Beschreibung</t>
   </si>
@@ -373,12 +373,27 @@
   <si>
     <t>M300 - LB3 - Selbsteinschätzung und Bewertung</t>
   </si>
+  <si>
+    <t>Genügend Kriterien erfüllt für 4 Punkte.</t>
+  </si>
+  <si>
+    <t>Alle Kriterien erfüllt. REF LB2</t>
+  </si>
+  <si>
+    <t>Genügend Kriterien erfüllt für 3 Punkte.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alle Kriterien erfüllt. Da Kubernetes keine Anleitung hatte und wir das selbstständig erarbeitet haben. </t>
+  </si>
+  <si>
+    <t>Zwei Kriterien erfüllt.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,11 +576,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1043,54 +1053,54 @@
     <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1234,23 +1244,23 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1258,27 +1268,27 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1286,47 +1296,47 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1342,31 +1352,31 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1378,13 +1388,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>659695</xdr:rowOff>
+          <xdr:rowOff>657225</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>194028</xdr:colOff>
+          <xdr:colOff>190500</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>857956</xdr:rowOff>
+          <xdr:rowOff>857250</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1416,11 +1426,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -1429,7 +1438,7 @@
             </a:extLst>
           </xdr:spPr>
         </xdr:sp>
-        <xdr:clientData/>
+        <xdr:clientData fLocksWithSheet="0"/>
       </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
@@ -1441,13 +1450,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>849313</xdr:rowOff>
+          <xdr:rowOff>847725</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>1049338</xdr:rowOff>
+          <xdr:rowOff>1047750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1457,7 +1466,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B993E47-42F5-DFB6-0CF3-2601E09F5B2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1479,11 +1488,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -1504,13 +1512,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>1040695</xdr:rowOff>
+          <xdr:rowOff>1038225</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>191558</xdr:colOff>
+          <xdr:colOff>190500</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>1240720</xdr:rowOff>
+          <xdr:rowOff>1238250</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1520,7 +1528,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36CE3766-F460-9CC0-7F2F-F6EF525116EB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1542,11 +1550,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -1567,13 +1574,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>1232077</xdr:rowOff>
+          <xdr:rowOff>1228725</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>191558</xdr:colOff>
+          <xdr:colOff>190500</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>1432102</xdr:rowOff>
+          <xdr:rowOff>1428750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1583,7 +1590,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E58FB91A-1BE7-97BC-6937-4FE72D2CD930}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1605,11 +1612,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -1630,13 +1636,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>1423458</xdr:rowOff>
+          <xdr:rowOff>1419225</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>191558</xdr:colOff>
+          <xdr:colOff>190500</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>1626205</xdr:rowOff>
+          <xdr:rowOff>1619250</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1646,7 +1652,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF784C10-B012-8CFB-7B41-EE0164BC5C0F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1668,11 +1674,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -1709,7 +1714,7 @@
                   <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C1A4217-560E-3624-7CB8-4BD0049EA5FF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1731,11 +1736,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -1756,13 +1760,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>804181</xdr:rowOff>
+          <xdr:rowOff>800100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>191861</xdr:colOff>
+          <xdr:colOff>190500</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>1004206</xdr:rowOff>
+          <xdr:rowOff>1000125</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1772,7 +1776,7 @@
                   <a14:compatExt spid="_x0000_s1034"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC2B9933-63B7-F550-830D-0DE1C694C4E4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1794,11 +1798,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -1819,13 +1822,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>994682</xdr:rowOff>
+          <xdr:rowOff>990600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>1194707</xdr:rowOff>
+          <xdr:rowOff>1190625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1835,7 +1838,7 @@
                   <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7007EE8D-3D02-7F59-944A-95C3F4224C95}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1857,11 +1860,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -1882,13 +1884,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>1185181</xdr:rowOff>
+          <xdr:rowOff>1181100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>191861</xdr:colOff>
+          <xdr:colOff>190500</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>1385206</xdr:rowOff>
+          <xdr:rowOff>1381125</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1898,7 +1900,7 @@
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27A4F23B-FA60-B290-10B5-90F26B13CB58}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1920,11 +1922,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -1945,13 +1946,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>1381124</xdr:rowOff>
+          <xdr:rowOff>1381125</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>191861</xdr:colOff>
+          <xdr:colOff>190500</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>1581149</xdr:rowOff>
+          <xdr:rowOff>1581150</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1961,7 +1962,7 @@
                   <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4478DFA8-B53A-39AD-AEC3-3CB3DC83AF68}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1983,11 +1984,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -2008,13 +2008,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>1947182</xdr:rowOff>
+          <xdr:rowOff>1943100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>191861</xdr:colOff>
+          <xdr:colOff>190500</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>2147207</xdr:rowOff>
+          <xdr:rowOff>2143125</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2024,7 +2024,7 @@
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB191899-5456-1B8D-D944-49ED84F98D81}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2046,11 +2046,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -2071,13 +2070,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>444954</xdr:rowOff>
+          <xdr:rowOff>447675</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>644979</xdr:rowOff>
+          <xdr:rowOff>647700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2087,7 +2086,7 @@
                   <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5313A5FE-CAB8-B3D7-5194-D2558321C86C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2109,11 +2108,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -2150,7 +2148,7 @@
                   <a14:compatExt spid="_x0000_s1052"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A235A3B-EC77-A588-F974-BEC2C4C32866}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2172,11 +2170,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -2213,7 +2210,7 @@
                   <a14:compatExt spid="_x0000_s1053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2073B97C-C8BE-7B32-1BB0-9B0F73BCC129}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2235,11 +2232,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -2276,7 +2272,7 @@
                   <a14:compatExt spid="_x0000_s1054"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E95EB1D-7F9D-0D73-DD8D-4C411D44800C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2298,11 +2294,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -2339,7 +2334,7 @@
                   <a14:compatExt spid="_x0000_s1055"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9341373-F139-C650-0B1D-B05C21FDA3C1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2361,11 +2356,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -2386,13 +2380,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>1549854</xdr:rowOff>
+          <xdr:rowOff>1552575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>1749879</xdr:rowOff>
+          <xdr:rowOff>1752600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2402,7 +2396,7 @@
                   <a14:compatExt spid="_x0000_s1056"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2A38614-10B0-5368-9F98-EE1AB1AEED97}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2424,11 +2418,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -2449,13 +2442,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>423252</xdr:rowOff>
+          <xdr:rowOff>419100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>623277</xdr:rowOff>
+          <xdr:rowOff>619125</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2465,7 +2458,7 @@
                   <a14:compatExt spid="_x0000_s1057"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0DD0811-89A6-53A2-43C9-A0FFB1192997}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2487,11 +2480,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -2512,13 +2504,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>1734911</xdr:rowOff>
+          <xdr:rowOff>1733550</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>1934936</xdr:rowOff>
+          <xdr:rowOff>1933575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2528,7 +2520,7 @@
                   <a14:compatExt spid="_x0000_s1059"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0361DAC4-87D9-FA47-5F2D-825598DA7D90}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2550,11 +2542,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -2591,7 +2582,7 @@
                   <a14:compatExt spid="_x0000_s1060"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E37B3AAB-C01E-7C2C-9400-89C28D4698F5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2613,11 +2604,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -2654,7 +2644,7 @@
                   <a14:compatExt spid="_x0000_s1061"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90C8340F-E714-1114-5F8F-AC8C4FFFC3EA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2676,11 +2666,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -2717,7 +2706,7 @@
                   <a14:compatExt spid="_x0000_s1062"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A7108C8-676B-A5D3-4C88-6F0242284D91}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2739,11 +2728,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -2770,7 +2758,7 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>1565275</xdr:rowOff>
+          <xdr:rowOff>1562100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2780,7 +2768,7 @@
                   <a14:compatExt spid="_x0000_s1064"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D687A4AF-2501-CBD6-42DE-F668C6896EAC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2802,11 +2790,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -2843,7 +2830,7 @@
                   <a14:compatExt spid="_x0000_s1065"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B78A6C5-D8D3-5C2E-E2BC-1A16B748DCE4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2865,11 +2852,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -2890,13 +2876,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>991380</xdr:rowOff>
+          <xdr:rowOff>990600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>193675</xdr:colOff>
+          <xdr:colOff>190500</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>1191405</xdr:rowOff>
+          <xdr:rowOff>1190625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2906,7 +2892,7 @@
                   <a14:compatExt spid="_x0000_s1097"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56222D55-B8E2-AE16-DD60-0E49503328A9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000049040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2928,11 +2914,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -2953,13 +2938,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>235530</xdr:rowOff>
+          <xdr:rowOff>238125</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>437105</xdr:rowOff>
+          <xdr:rowOff>438150</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2969,7 +2954,7 @@
                   <a14:compatExt spid="_x0000_s1098"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{933FD475-E2A5-DD15-4491-58C12896E54A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2991,11 +2976,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -3016,13 +3000,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>429068</xdr:rowOff>
+          <xdr:rowOff>428625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>189835</xdr:colOff>
+          <xdr:colOff>190500</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>630201</xdr:rowOff>
+          <xdr:rowOff>628650</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3032,7 +3016,7 @@
                   <a14:compatExt spid="_x0000_s1099"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95B95825-7AB5-FE00-E2EF-F4D48C4F6E63}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3054,11 +3038,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -3079,13 +3062,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>634757</xdr:rowOff>
+          <xdr:rowOff>638175</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>189835</xdr:colOff>
+          <xdr:colOff>190500</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>835890</xdr:rowOff>
+          <xdr:rowOff>838200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3095,7 +3078,7 @@
                   <a14:compatExt spid="_x0000_s1100"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A281563-E121-906B-60C4-89034779730D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3117,11 +3100,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -3142,13 +3124,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>1074616</xdr:rowOff>
+          <xdr:rowOff>1076325</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>189835</xdr:colOff>
+          <xdr:colOff>190500</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>1275749</xdr:rowOff>
+          <xdr:rowOff>1276350</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3158,7 +3140,7 @@
                   <a14:compatExt spid="_x0000_s1101"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DD7B901-A608-B981-A7B1-2357E483F313}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3180,11 +3162,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -3205,13 +3186,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>1254989</xdr:rowOff>
+          <xdr:rowOff>1257300</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>189835</xdr:colOff>
+          <xdr:colOff>190500</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>1456122</xdr:rowOff>
+          <xdr:rowOff>1457325</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3221,7 +3202,7 @@
                   <a14:compatExt spid="_x0000_s1102"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{631B534D-CB21-4021-84DB-9B048DE9BDCF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3243,11 +3224,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -3268,13 +3248,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>420863</xdr:rowOff>
+          <xdr:rowOff>419100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>188031</xdr:colOff>
+          <xdr:colOff>190500</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>622652</xdr:rowOff>
+          <xdr:rowOff>619125</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3284,7 +3264,7 @@
                   <a14:compatExt spid="_x0000_s1103"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDD25185-0C95-D110-170C-AACD6E21A9C7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3306,11 +3286,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -3331,13 +3310,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>815974</xdr:rowOff>
+          <xdr:rowOff>819150</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>188031</xdr:colOff>
+          <xdr:colOff>190500</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>1017763</xdr:rowOff>
+          <xdr:rowOff>1019175</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3347,7 +3326,7 @@
                   <a14:compatExt spid="_x0000_s1104"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72089EDC-B46A-0F2C-4067-6B5C132BDEC6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000050040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3369,11 +3348,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -3394,13 +3372,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>1196975</xdr:rowOff>
+          <xdr:rowOff>1200150</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>188031</xdr:colOff>
+          <xdr:colOff>190500</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>1398764</xdr:rowOff>
+          <xdr:rowOff>1400175</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3410,7 +3388,7 @@
                   <a14:compatExt spid="_x0000_s1105"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99EFF58E-5CAD-8E6B-9A32-E1BE6E6C9311}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000051040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3432,11 +3410,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -3457,13 +3434,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>230364</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>188031</xdr:colOff>
+          <xdr:colOff>190500</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>432153</xdr:rowOff>
+          <xdr:rowOff>428625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3473,7 +3450,7 @@
                   <a14:compatExt spid="_x0000_s1106"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EDD3668-4D5B-A38C-7DBE-1EEDAD3D4FCA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000052040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3495,11 +3472,10 @@
             </a:ln>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -3546,7 +3522,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3856,11 +3832,11 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="71.42578125" style="5" customWidth="1"/>
@@ -3913,7 +3889,9 @@
       <c r="B4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="18"/>
+      <c r="C4" s="18">
+        <v>4</v>
+      </c>
       <c r="D4" s="17" t="str">
         <f>IF(Table1[[#This Row],[Punkte 
 Bewertung Lehrperson
@@ -3924,7 +3902,9 @@
 1-4]],1,2))</f>
         <v/>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="11" t="s">
+        <v>18</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="7"/>
       <c r="H4" s="14"/>
@@ -3933,7 +3913,9 @@
       <c r="B5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="18"/>
+      <c r="C5" s="18">
+        <v>4</v>
+      </c>
       <c r="D5" s="17" t="str">
         <f>IF(Table1[[#This Row],[Punkte 
 Bewertung Lehrperson
@@ -3944,7 +3926,9 @@
 1-4]],1,2))</f>
         <v/>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="11" t="s">
+        <v>18</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="7"/>
       <c r="H5" s="14"/>
@@ -3953,7 +3937,9 @@
       <c r="B6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="18"/>
+      <c r="C6" s="18">
+        <v>4</v>
+      </c>
       <c r="D6" s="17" t="str">
         <f>IF(Table1[[#This Row],[Punkte 
 Bewertung Lehrperson
@@ -3964,7 +3950,9 @@
 1-4]],1,2))</f>
         <v/>
       </c>
-      <c r="E6" s="13"/>
+      <c r="E6" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="12"/>
       <c r="H6" s="14"/>
@@ -3973,7 +3961,9 @@
       <c r="B7" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="18"/>
+      <c r="C7" s="18">
+        <v>3</v>
+      </c>
       <c r="D7" s="17" t="str">
         <f>IF(Table1[[#This Row],[Punkte 
 Bewertung Lehrperson
@@ -3984,7 +3974,9 @@
 1-4]],1,2))</f>
         <v/>
       </c>
-      <c r="E7" s="13"/>
+      <c r="E7" s="13" t="s">
+        <v>19</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="12"/>
       <c r="H7" s="14"/>
@@ -3993,7 +3985,9 @@
       <c r="B8" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="18">
+        <v>4</v>
+      </c>
       <c r="D8" s="17" t="str">
         <f>IF(Table1[[#This Row],[Punkte 
 Bewertung Lehrperson
@@ -4004,7 +3998,9 @@
 1-4]],1,2))</f>
         <v/>
       </c>
-      <c r="E8" s="13"/>
+      <c r="E8" s="13" t="s">
+        <v>20</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="12"/>
       <c r="H8" s="14"/>
@@ -4014,7 +4010,9 @@
       <c r="B9" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="18"/>
+      <c r="C9" s="18">
+        <v>2</v>
+      </c>
       <c r="D9" s="17" t="str">
         <f>IF(Table1[[#This Row],[Punkte 
 Bewertung Lehrperson
@@ -4025,7 +4023,9 @@
 1-4]],1,2))</f>
         <v/>
       </c>
-      <c r="E9" s="13"/>
+      <c r="E9" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="F9" s="3"/>
       <c r="G9" s="12"/>
       <c r="H9" s="14"/>
@@ -4038,7 +4038,7 @@
         <f>SUM(Table1[Punkte
 Selbsteinschätzung
 1-4])</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="10"/>
@@ -4051,7 +4051,7 @@
       <c r="G10" s="10"/>
       <c r="H10" s="2">
         <f>IF(F10=0,ROUND(C10*5/24+1,1),ROUND(F10*5/24+1,1))</f>
-        <v>1</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25"/>
@@ -5000,6 +5000,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ReferenceId xmlns="f64e2662-c046-4068-9eb0-783a67eee65e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5008,22 +5016,38 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ReferenceId xmlns="f64e2662-c046-4068-9eb0-783a67eee65e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61106B5B-B16E-471C-9AB2-3A2D5F6BAE60}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61106B5B-B16E-471C-9AB2-3A2D5F6BAE60}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f64e2662-c046-4068-9eb0-783a67eee65e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C88061-89EB-4B2A-86EF-F4D06CD28E61}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1975346D-1BEC-478D-8DAF-EEE5E87C2B18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f64e2662-c046-4068-9eb0-783a67eee65e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1975346D-1BEC-478D-8DAF-EEE5E87C2B18}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C88061-89EB-4B2A-86EF-F4D06CD28E61}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>